<commit_message>
Refactored the script to handle the popups in the facebook application
</commit_message>
<xml_diff>
--- a/Seleniumfacebook/TestDataAccess/TestData.xlsx
+++ b/Seleniumfacebook/TestDataAccess/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\source\repos\Seleniumfacebook\Seleniumfacebook\TestDataAccess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347F1E49-BD40-4060-AFEF-C25235A692E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1B89AC-CE54-4C01-9D81-975D10B10429}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>TestLoginAndLogout</t>
   </si>
   <si>
-    <t>Rajesh</t>
+    <t>Rajeshr</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,7 +396,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>9542030759</v>
+        <v>8074453962</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>

</xml_diff>